<commit_message>
this is the evaluations on runtimes for runtime.js
</commit_message>
<xml_diff>
--- a/runtime-evaluation.xlsx
+++ b/runtime-evaluation.xlsx
@@ -266,11 +266,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="179077504"/>
-        <c:axId val="179079040"/>
+        <c:axId val="258642688"/>
+        <c:axId val="258644224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179077504"/>
+        <c:axId val="258642688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +279,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179079040"/>
+        <c:crossAx val="258644224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -287,7 +287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179079040"/>
+        <c:axId val="258644224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -298,7 +298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179077504"/>
+        <c:crossAx val="258642688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +645,7 @@
   <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>